<commit_message>
Merged PR 10873: Rates effective 9/1
Related work items: #32986
</commit_message>
<xml_diff>
--- a/ApolloQA/Data/RatingManual/GA/DT.3.xlsx
+++ b/ApolloQA/Data/RatingManual/GA/DT.3.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DT.3" sheetId="1" r:id="Rf78cfea173ce46d1"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DT.3" sheetId="1" r:id="Rb58cf1a67f644e43"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -12,79 +12,82 @@
   <x:sheetData>
     <x:row>
       <x:c t="str">
-        <x:v>Driver Rating Plan</x:v>
+        <x:v>Limit</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>Minimum Decrease</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>Minimum Increase</x:v>
+        <x:v>Excess Limits Rating Factor</x:v>
       </x:c>
     </x:row>
     <x:row>
       <x:c t="str">
-        <x:v>Fleet</x:v>
+        <x:v>$1,200,000</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>-25.00%</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>25.00%</x:v>
+        <x:v>1.1250</x:v>
       </x:c>
     </x:row>
     <x:row>
       <x:c t="str">
-        <x:v>For Hire Public</x:v>
+        <x:v>$1,500,000</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>-10.00%</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>10.00%</x:v>
+        <x:v>1.3000</x:v>
       </x:c>
     </x:row>
     <x:row>
       <x:c t="str">
-        <x:v>Livery</x:v>
+        <x:v>$2,000,000</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>-10.00%</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>10.00%</x:v>
+        <x:v>1.4500</x:v>
       </x:c>
     </x:row>
     <x:row>
       <x:c t="str">
-        <x:v>Standard</x:v>
+        <x:v>$2,500,000</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>-25.00%</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>25.00%</x:v>
+        <x:v>1.6300</x:v>
       </x:c>
     </x:row>
     <x:row>
       <x:c t="str">
-        <x:v>Trucker</x:v>
+        <x:v>$3,000,000</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>-10.00%</x:v>
-      </x:c>
-      <x:c t="str">
-        <x:v>10.00%</x:v>
+        <x:v>1.7500</x:v>
       </x:c>
     </x:row>
     <x:row>
       <x:c t="str">
-        <x:v>Unity</x:v>
+        <x:v>$3,500,000</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>-25.00%</x:v>
+        <x:v>1.8700</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>$4,000,000</x:v>
       </x:c>
       <x:c t="str">
-        <x:v>25.00%</x:v>
+        <x:v>1.9500</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>$4,500,000</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2.0400</x:v>
+      </x:c>
+    </x:row>
+    <x:row>
+      <x:c t="str">
+        <x:v>$5,000,000</x:v>
+      </x:c>
+      <x:c t="str">
+        <x:v>2.1000</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>